<commit_message>
- Updated with addictions and dementia data
</commit_message>
<xml_diff>
--- a/bibliometrics.xlsx
+++ b/bibliometrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/NM_Movement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="8_{43F4D15B-8EC9-42D5-A0FD-8DB7B45422F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08D62A5-BC5D-494C-99E4-F7693CE8B9A1}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{43F4D15B-8EC9-42D5-A0FD-8DB7B45422F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63C51902-6B98-456C-9994-997E5ABB4941}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" activeTab="1" xr2:uid="{BFE7E20A-D837-4AFE-BD2B-7EE1BDE7347C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BFE7E20A-D837-4AFE-BD2B-7EE1BDE7347C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$C$1</c15:sqref>
@@ -636,7 +636,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -680,7 +680,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$C$2:$C$11</c15:sqref>
@@ -723,7 +723,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-620C-4346-B69A-8D0216147B25}"/>
                   </c:ext>
@@ -736,7 +736,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$D$1</c15:sqref>
@@ -763,7 +763,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -807,7 +807,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$D$2:$D$11</c15:sqref>
@@ -850,7 +850,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-620C-4346-B69A-8D0216147B25}"/>
                   </c:ext>
@@ -863,7 +863,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$E$1</c15:sqref>
@@ -890,7 +890,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -934,7 +934,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$E$2:$E$11</c15:sqref>
@@ -977,7 +977,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-620C-4346-B69A-8D0216147B25}"/>
                   </c:ext>
@@ -990,7 +990,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$H$1</c15:sqref>
@@ -1017,7 +1017,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -1061,7 +1061,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$H$2:$H$11</c15:sqref>
@@ -1104,7 +1104,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-620C-4346-B69A-8D0216147B25}"/>
                   </c:ext>
@@ -1117,7 +1117,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$I$1</c15:sqref>
@@ -1144,7 +1144,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -1188,7 +1188,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$I$2:$I$11</c15:sqref>
@@ -1231,7 +1231,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-620C-4346-B69A-8D0216147B25}"/>
                   </c:ext>
@@ -2048,7 +2048,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$D$1</c15:sqref>
@@ -2075,7 +2075,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$A$2:$A$11</c15:sqref>
@@ -2119,7 +2119,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Overall!$D$2:$D$11</c15:sqref>
@@ -2162,7 +2162,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-1477-4859-B61F-A69216246CFA}"/>
                   </c:ext>
@@ -5337,15 +5337,15 @@
         <v>5024</v>
       </c>
       <c r="H2">
-        <f>C2/$B2*100</f>
+        <f t="shared" ref="H2:H11" si="0">C2/$B2*100</f>
         <v>3.0935200400085732</v>
       </c>
       <c r="I2">
-        <f>D2/$B2*100</f>
+        <f t="shared" ref="I2:I11" si="1">D2/$B2*100</f>
         <v>40.655140387225835</v>
       </c>
       <c r="J2">
-        <f>E2/$B2*100</f>
+        <f t="shared" ref="J2:J11" si="2">E2/$B2*100</f>
         <v>22.708437522326214</v>
       </c>
       <c r="K2">
@@ -5374,31 +5374,31 @@
         <v>1905</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="0">E3-C3</f>
+        <f t="shared" ref="F3:F11" si="3">E3-C3</f>
         <v>1715</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="1">D3-E3</f>
+        <f t="shared" ref="G3:G11" si="4">D3-E3</f>
         <v>1259</v>
       </c>
       <c r="H3">
-        <f>C3/$B3*100</f>
+        <f t="shared" si="0"/>
         <v>2.7460615695909811</v>
       </c>
       <c r="I3">
-        <f>D3/$B3*100</f>
+        <f t="shared" si="1"/>
         <v>45.729151611504555</v>
       </c>
       <c r="J3">
-        <f>E3/$B3*100</f>
+        <f t="shared" si="2"/>
         <v>27.532880474056942</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K11" si="2">J3-H3</f>
+        <f t="shared" ref="K3:K11" si="5">J3-H3</f>
         <v>24.78681890446596</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L11" si="3">I3-J3</f>
+        <f t="shared" ref="L3:L11" si="6">I3-J3</f>
         <v>18.196271137447614</v>
       </c>
     </row>
@@ -5419,31 +5419,31 @@
         <v>3506</v>
       </c>
       <c r="F4">
+        <f t="shared" si="3"/>
+        <v>2863</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>3634</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
-        <v>2863</v>
-      </c>
-      <c r="G4">
+        <v>3.3252314216269325</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="1"/>
-        <v>3634</v>
-      </c>
-      <c r="H4">
-        <f>C4/$B4*100</f>
-        <v>3.3252314216269325</v>
-      </c>
-      <c r="I4">
-        <f>D4/$B4*100</f>
         <v>36.924031649169983</v>
       </c>
       <c r="J4">
-        <f>E4/$B4*100</f>
+        <f t="shared" si="2"/>
         <v>18.131044112323526</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>14.805812690696593</v>
       </c>
       <c r="L4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>18.792987536846457</v>
       </c>
     </row>
@@ -5464,31 +5464,31 @@
         <v>839</v>
       </c>
       <c r="F5">
+        <f t="shared" si="3"/>
+        <v>775</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>382</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>775</v>
-      </c>
-      <c r="G5">
+        <v>2.3503488799118619</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="1"/>
-        <v>382</v>
-      </c>
-      <c r="H5">
-        <f>C5/$B5*100</f>
-        <v>2.3503488799118619</v>
-      </c>
-      <c r="I5">
-        <f>D5/$B5*100</f>
         <v>44.840249724568494</v>
       </c>
       <c r="J5">
-        <f>E5/$B5*100</f>
+        <f t="shared" si="2"/>
         <v>30.811604847594566</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>28.461255967682703</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14.028644876973928</v>
       </c>
     </row>
@@ -5509,31 +5509,31 @@
         <v>1978</v>
       </c>
       <c r="F6">
+        <f t="shared" si="3"/>
+        <v>1758</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>1801</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>1758</v>
-      </c>
-      <c r="G6">
+        <v>2.4583752374566994</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
-        <v>1801</v>
-      </c>
-      <c r="H6">
-        <f>C6/$B6*100</f>
-        <v>2.4583752374566994</v>
-      </c>
-      <c r="I6">
-        <f>D6/$B6*100</f>
         <v>42.228181919767572</v>
       </c>
       <c r="J6">
-        <f>E6/$B6*100</f>
+        <f t="shared" si="2"/>
         <v>22.103028271315232</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>19.644653033858532</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20.12515364845234</v>
       </c>
     </row>
@@ -5554,31 +5554,31 @@
         <v>716</v>
       </c>
       <c r="F7">
+        <f t="shared" si="3"/>
+        <v>646</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>481</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>646</v>
-      </c>
-      <c r="G7">
+        <v>2.3704707077548255</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="1"/>
-        <v>481</v>
-      </c>
-      <c r="H7">
-        <f>C7/$B7*100</f>
-        <v>2.3704707077548255</v>
-      </c>
-      <c r="I7">
-        <f>D7/$B7*100</f>
         <v>40.535049102607516</v>
       </c>
       <c r="J7">
-        <f>E7/$B7*100</f>
+        <f t="shared" si="2"/>
         <v>24.246528953606504</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>21.876058245851677</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16.288520149001013</v>
       </c>
     </row>
@@ -5599,31 +5599,31 @@
         <v>204</v>
       </c>
       <c r="F8">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-      <c r="G8">
+        <v>3.8135593220338984</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="H8">
-        <f>C8/$B8*100</f>
-        <v>3.8135593220338984</v>
-      </c>
-      <c r="I8">
-        <f>D8/$B8*100</f>
         <v>57.627118644067799</v>
       </c>
       <c r="J8">
-        <f>E8/$B8*100</f>
+        <f t="shared" si="2"/>
         <v>43.220338983050851</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>39.406779661016955</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14.406779661016948</v>
       </c>
     </row>
@@ -5644,31 +5644,31 @@
         <v>641</v>
       </c>
       <c r="F9">
+        <f t="shared" si="3"/>
+        <v>586</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>352</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>586</v>
-      </c>
-      <c r="G9">
+        <v>2.4619516562220234</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
-        <v>352</v>
-      </c>
-      <c r="H9">
-        <f>C9/$B9*100</f>
-        <v>2.4619516562220234</v>
-      </c>
-      <c r="I9">
-        <f>D9/$B9*100</f>
         <v>44.449418084153983</v>
       </c>
       <c r="J9">
-        <f>E9/$B9*100</f>
+        <f t="shared" si="2"/>
         <v>28.692927484333037</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>26.230975828111013</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>15.756490599820946</v>
       </c>
     </row>
@@ -5689,31 +5689,31 @@
         <v>167</v>
       </c>
       <c r="F10">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>162</v>
-      </c>
-      <c r="G10">
+        <v>1.5151515151515151</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="H10">
-        <f>C10/$B10*100</f>
-        <v>1.5151515151515151</v>
-      </c>
-      <c r="I10">
-        <f>D10/$B10*100</f>
         <v>60.606060606060609</v>
       </c>
       <c r="J10">
-        <f>E10/$B10*100</f>
+        <f t="shared" si="2"/>
         <v>50.606060606060609</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>49.090909090909093</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
     </row>
@@ -5734,31 +5734,31 @@
         <v>46</v>
       </c>
       <c r="F11">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="G11">
+        <v>7.6923076923076925</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <f>C11/$B11*100</f>
-        <v>7.6923076923076925</v>
-      </c>
-      <c r="I11">
-        <f>D11/$B11*100</f>
         <v>70.329670329670336</v>
       </c>
       <c r="J11">
-        <f>E11/$B11*100</f>
+        <f t="shared" si="2"/>
         <v>50.549450549450547</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>42.857142857142854</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>19.780219780219788</v>
       </c>
     </row>
@@ -5779,31 +5779,31 @@
         <v>2210</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F16" si="4">E13-C13</f>
+        <f t="shared" ref="F13:F16" si="7">E13-C13</f>
         <v>1985</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G16" si="5">D13-E13</f>
+        <f t="shared" ref="G13:G16" si="8">D13-E13</f>
         <v>1517</v>
       </c>
       <c r="H13">
-        <f>C13/$B13*100</f>
+        <f t="shared" ref="H13:J19" si="9">C13/$B13*100</f>
         <v>2.6096033402922756</v>
       </c>
       <c r="I13">
-        <f>D13/$B13*100</f>
+        <f t="shared" si="9"/>
         <v>43.226629552308047</v>
       </c>
       <c r="J13">
-        <f>E13/$B13*100</f>
+        <f t="shared" si="9"/>
         <v>25.632103920204131</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K16" si="6">J13-H13</f>
+        <f t="shared" ref="K13:K16" si="10">J13-H13</f>
         <v>23.022500579911856</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:L16" si="7">I13-J13</f>
+        <f t="shared" ref="L13:L16" si="11">I13-J13</f>
         <v>17.594525632103917</v>
       </c>
     </row>
@@ -5824,31 +5824,31 @@
         <v>4246</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3441</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3803</v>
       </c>
       <c r="H14">
-        <f>C14/$B14*100</f>
+        <f t="shared" si="9"/>
         <v>4.4891813517733654</v>
       </c>
       <c r="I14">
-        <f>D14/$B14*100</f>
+        <f t="shared" si="9"/>
         <v>44.886236894936424</v>
       </c>
       <c r="J14">
-        <f>E14/$B14*100</f>
+        <f t="shared" si="9"/>
         <v>23.678340397055546</v>
       </c>
       <c r="K14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>19.189159045282182</v>
       </c>
       <c r="L14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>21.207896497880878</v>
       </c>
     </row>
@@ -5869,31 +5869,31 @@
         <v>1241</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1042</v>
       </c>
       <c r="G15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1346</v>
       </c>
       <c r="H15">
-        <f>C15/$B15*100</f>
+        <f t="shared" si="9"/>
         <v>3.4452908587257616</v>
       </c>
       <c r="I15">
-        <f>D15/$B15*100</f>
+        <f t="shared" si="9"/>
         <v>44.788781163434905</v>
       </c>
       <c r="J15">
-        <f>E15/$B15*100</f>
+        <f t="shared" si="9"/>
         <v>21.485457063711909</v>
       </c>
       <c r="K15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>18.040166204986146</v>
       </c>
       <c r="L15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>23.303324099722996</v>
       </c>
     </row>
@@ -5914,31 +5914,31 @@
         <v>425</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>360</v>
       </c>
       <c r="G16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>384</v>
       </c>
       <c r="H16">
-        <f>C16/$B16*100</f>
+        <f t="shared" si="9"/>
         <v>3.3265097236438077</v>
       </c>
       <c r="I16">
-        <f>D16/$B16*100</f>
+        <f t="shared" si="9"/>
         <v>41.402251791197543</v>
       </c>
       <c r="J16">
-        <f>E16/$B16*100</f>
+        <f t="shared" si="9"/>
         <v>21.750255885363355</v>
       </c>
       <c r="K16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>18.423746161719549</v>
       </c>
       <c r="L16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>19.651995905834188</v>
       </c>
     </row>
@@ -5959,31 +5959,31 @@
         <v>2401</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F19" si="8">E17-C17</f>
+        <f t="shared" ref="F17:F19" si="12">E17-C17</f>
         <v>2327</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G19" si="9">D17-E17</f>
+        <f t="shared" ref="G17:G19" si="13">D17-E17</f>
         <v>1443</v>
       </c>
       <c r="H17">
-        <f>C17/$B17*100</f>
+        <f t="shared" si="9"/>
         <v>0.65469344421834907</v>
       </c>
       <c r="I17">
-        <f>D17/$B17*100</f>
+        <f t="shared" si="9"/>
         <v>34.008670264531546</v>
       </c>
       <c r="J17">
-        <f>E17/$B17*100</f>
+        <f t="shared" si="9"/>
         <v>21.242148102273735</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K19" si="10">J17-H17</f>
+        <f t="shared" ref="K17:K19" si="14">J17-H17</f>
         <v>20.587454658055385</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L19" si="11">I17-J17</f>
+        <f t="shared" ref="L17:L19" si="15">I17-J17</f>
         <v>12.766522162257811</v>
       </c>
     </row>
@@ -6004,31 +6004,31 @@
         <v>837</v>
       </c>
       <c r="F18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>816</v>
       </c>
       <c r="G18">
+        <f t="shared" si="13"/>
+        <v>533</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="9"/>
-        <v>533</v>
-      </c>
-      <c r="H18">
-        <f>C18/$B18*100</f>
         <v>0.58577405857740583</v>
       </c>
       <c r="I18">
-        <f>D18/$B18*100</f>
+        <f t="shared" si="9"/>
         <v>38.214783821478385</v>
       </c>
       <c r="J18">
-        <f>E18/$B18*100</f>
+        <f t="shared" si="9"/>
         <v>23.347280334728033</v>
       </c>
       <c r="K18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>22.761506276150627</v>
       </c>
       <c r="L18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>14.867503486750351</v>
       </c>
     </row>
@@ -6049,31 +6049,31 @@
         <v>327</v>
       </c>
       <c r="F19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>321</v>
       </c>
       <c r="G19">
+        <f t="shared" si="13"/>
+        <v>117</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="9"/>
-        <v>117</v>
-      </c>
-      <c r="H19">
-        <f>C19/$B19*100</f>
         <v>0.51502145922746778</v>
       </c>
       <c r="I19">
-        <f>D19/$B19*100</f>
+        <f t="shared" si="9"/>
         <v>38.111587982832617</v>
       </c>
       <c r="J19">
-        <f>E19/$B19*100</f>
+        <f t="shared" si="9"/>
         <v>28.068669527896994</v>
       </c>
       <c r="K19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>27.553648068669524</v>
       </c>
       <c r="L19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>10.042918454935624</v>
       </c>
     </row>
@@ -6088,11 +6088,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CC9BEB-09D1-4BC4-B989-43DD9A11B1FC}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">

</xml_diff>